<commit_message>
Oracle can now identify items.
</commit_message>
<xml_diff>
--- a/SpellSuccessPercentage.xlsx
+++ b/SpellSuccessPercentage.xlsx
@@ -392,7 +392,7 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,20 +402,20 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2">
         <f>G2*H2</f>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
@@ -423,20 +423,20 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3">
         <f>G3*H3</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -445,16 +445,16 @@
       </c>
       <c r="C4">
         <f>I9</f>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f>G4*H4</f>
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -475,11 +475,11 @@
         <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <f>G5*H5</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -496,11 +496,11 @@
         <v>6</v>
       </c>
       <c r="H6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>G6*H6</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
@@ -511,11 +511,11 @@
         <v>2</v>
       </c>
       <c r="H7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f>G7*H7</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
@@ -524,7 +524,7 @@
       </c>
       <c r="C8">
         <f>(C2-3)*10</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -534,14 +534,14 @@
       </c>
       <c r="C9">
         <f>D9*(C3-1)</f>
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>-45</v>
       </c>
       <c r="I9">
         <f>SUM(I2:I8)</f>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
       </c>
       <c r="C10">
         <f>D10*C4</f>
-        <v>-145</v>
+        <v>-115</v>
       </c>
       <c r="D10">
         <v>-5</v>
@@ -562,11 +562,11 @@
       </c>
       <c r="C11">
         <f>D11*(C5-1)</f>
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <f>($C$2-3)*3</f>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
@@ -575,11 +575,11 @@
       </c>
       <c r="C12">
         <f>D12*C6</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <f>($C$2-3)*3</f>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
       </c>
       <c r="C14">
         <f>SUM(C8:C13)</f>
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small oracle improvements; fountain appears in 1 in 20 rooms
</commit_message>
<xml_diff>
--- a/SpellSuccessPercentage.xlsx
+++ b/SpellSuccessPercentage.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Spell level</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Int/Wis</t>
+  </si>
+  <si>
+    <t>Spell cost</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,7 +405,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -414,7 +417,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f>G2*H2</f>
+        <f t="shared" ref="I2:I7" si="0">G2*H2</f>
         <v>1</v>
       </c>
     </row>
@@ -423,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -432,11 +435,11 @@
         <v>10</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <f>G3*H3</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -445,7 +448,7 @@
       </c>
       <c r="C4">
         <f>I9</f>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -457,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f>G4*H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -466,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -475,11 +478,11 @@
         <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f>G5*H5</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -487,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -499,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <f>G6*H6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -511,11 +514,11 @@
         <v>2</v>
       </c>
       <c r="H7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <f>G7*H7</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
@@ -524,7 +527,7 @@
       </c>
       <c r="C8">
         <f>(C2-3)*10</f>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -534,14 +537,14 @@
       </c>
       <c r="C9">
         <f>D9*(C3-1)</f>
-        <v>0</v>
+        <v>-1080</v>
       </c>
       <c r="D9">
         <v>-45</v>
       </c>
       <c r="I9">
         <f>SUM(I2:I8)</f>
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -550,7 +553,7 @@
       </c>
       <c r="C10">
         <f>D10*C4</f>
-        <v>-115</v>
+        <v>-5</v>
       </c>
       <c r="D10">
         <v>-5</v>
@@ -562,11 +565,18 @@
       </c>
       <c r="C11">
         <f>D11*(C5-1)</f>
-        <v>42</v>
+        <v>900</v>
       </c>
       <c r="D11">
         <f>($C$2-3)*3</f>
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <f>C3*3</f>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
@@ -575,11 +585,11 @@
       </c>
       <c r="C12">
         <f>D12*C6</f>
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="D12">
         <f>($C$2-3)*3</f>
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -588,7 +598,7 @@
       </c>
       <c r="C14">
         <f>SUM(C8:C13)</f>
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spell success percentage updated, as per Tommi's suggestion.
</commit_message>
<xml_diff>
--- a/SpellSuccessPercentage.xlsx
+++ b/SpellSuccessPercentage.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Spell level</t>
   </si>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,7 +405,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -414,11 +414,11 @@
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I7" si="0">G2*H2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
@@ -426,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -448,7 +448,7 @@
       </c>
       <c r="C4">
         <f>I9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -469,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -490,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -526,78 +526,87 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <f>(C2-3)*10</f>
-        <v>150</v>
+        <v>-210</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <f>D9*(C3-1)</f>
-        <v>-1080</v>
+        <f>(C2)*D9</f>
+        <v>260</v>
       </c>
       <c r="D9">
-        <v>-45</v>
+        <v>20</v>
       </c>
       <c r="I9">
         <f>SUM(I2:I8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f>D10*C4</f>
-        <v>-5</v>
+        <f>D10*(C3)</f>
+        <v>-20</v>
       </c>
       <c r="D10">
-        <v>-5</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <f>D11*(C5-1)</f>
-        <v>900</v>
+        <f>D11*C4</f>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f>($C$2-3)*3</f>
-        <v>45</v>
+        <v>-5</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
       </c>
       <c r="G11">
         <f>C3*3</f>
-        <v>75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <f>D12*(C5)</f>
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
-        <f>D12*C6</f>
-        <v>135</v>
-      </c>
-      <c r="D12">
-        <f>($C$2-3)*3</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="C13">
+        <f>D13*C6</f>
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
-        <f>SUM(C8:C13)</f>
+      <c r="C15">
+        <f>SUM(C8:C14)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>